<commit_message>
attendance new route added
</commit_message>
<xml_diff>
--- a/bill docs/22SNCJO-373/attendance/attendance_format_3_2024.xlsx
+++ b/bill docs/22SNCJO-373/attendance/attendance_format_3_2024.xlsx
@@ -2853,10 +2853,10 @@
         </is>
       </c>
       <c r="D9" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F9" s="330" t="inlineStr">
         <is>
@@ -2864,22 +2864,22 @@
         </is>
       </c>
       <c r="G9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K9" s="327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M9" s="330" t="inlineStr">
         <is>
@@ -2887,22 +2887,22 @@
         </is>
       </c>
       <c r="N9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S9" s="329" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="T9" s="330" t="inlineStr">
         <is>
@@ -2910,22 +2910,22 @@
         </is>
       </c>
       <c r="U9" s="327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9" s="327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9" s="327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9" s="327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9" s="330" t="inlineStr">
         <is>
@@ -2933,22 +2933,22 @@
         </is>
       </c>
       <c r="AB9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AC9" s="327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD9" s="327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AF9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AG9" s="327" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH9" s="330" t="inlineStr">
         <is>
@@ -2956,7 +2956,7 @@
         </is>
       </c>
       <c r="AI9" s="329" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="AJ9" s="327" t="n">
         <v>1</v>
@@ -2977,10 +2977,10 @@
         </is>
       </c>
       <c r="D10" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="332" t="inlineStr">
         <is>
@@ -2991,7 +2991,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="329" t="n">
         <v>1</v>
@@ -3014,42 +3014,40 @@
         <v>1</v>
       </c>
       <c r="O10" s="329" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="329" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="329" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="329" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="329" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" s="332" t="n">
         <v>1</v>
       </c>
-      <c r="P10" s="329" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="329" t="n">
-        <v>1</v>
-      </c>
-      <c r="R10" s="329" t="n">
-        <v>1</v>
-      </c>
-      <c r="S10" s="329" t="n">
-        <v>1</v>
-      </c>
-      <c r="T10" s="332" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
       <c r="U10" s="329" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="V10" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X10" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA10" s="332" t="inlineStr">
         <is>
@@ -3060,27 +3058,25 @@
         <v>1</v>
       </c>
       <c r="AC10" s="329" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="329" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="329" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AF10" s="329" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="329" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="332" t="n">
         <v>1</v>
       </c>
-      <c r="AD10" s="329" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="329" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="329" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="329" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH10" s="332" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
       <c r="AI10" s="329" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="AJ10" s="329" t="n">
         <v>1</v>
@@ -3141,7 +3137,7 @@
         <v>1</v>
       </c>
       <c r="P11" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="329" t="n">
         <v>1</v>
@@ -3152,10 +3148,8 @@
       <c r="S11" s="329" t="n">
         <v>1</v>
       </c>
-      <c r="T11" s="332" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
+      <c r="T11" s="332" t="n">
+        <v>0.5</v>
       </c>
       <c r="U11" s="329" t="n">
         <v>1</v>
@@ -3164,7 +3158,7 @@
         <v>1</v>
       </c>
       <c r="W11" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X11" s="329" t="n">
         <v>1</v>
@@ -3173,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="Z11" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA11" s="332" t="inlineStr">
         <is>
@@ -3184,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="AC11" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD11" s="329" t="n">
         <v>1</v>
@@ -3193,10 +3187,10 @@
         <v>1</v>
       </c>
       <c r="AF11" s="329" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AG11" s="329" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH11" s="332" t="inlineStr">
         <is>
@@ -3204,7 +3198,7 @@
         </is>
       </c>
       <c r="AI11" s="329" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="AJ11" s="329" t="n">
         <v>1</v>
@@ -3296,7 +3290,7 @@
       <c r="AG13" s="335" t="n"/>
       <c r="AH13" s="336" t="n"/>
       <c r="AI13" s="329" t="n">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="AJ13" s="329" t="n">
         <v>0</v>
@@ -3713,7 +3707,7 @@
         </is>
       </c>
       <c r="C6" s="352" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D6" s="352" t="n">
         <v>1</v>
@@ -3722,43 +3716,43 @@
         <v>709</v>
       </c>
       <c r="F6" s="352" t="n">
-        <v>18434</v>
+        <v>5672</v>
       </c>
       <c r="G6" s="352" t="n">
         <v>709</v>
       </c>
       <c r="H6" s="352" t="n">
-        <v>15000</v>
+        <v>5672</v>
       </c>
       <c r="I6" s="352" t="n">
-        <v>1800</v>
+        <v>680.64</v>
       </c>
       <c r="J6" s="352" t="n">
-        <v>138.26</v>
+        <v>42.54</v>
       </c>
       <c r="K6" s="352" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="352" t="n">
-        <v>1938.26</v>
+        <v>723.1799999999999</v>
       </c>
       <c r="M6" s="352" t="n">
-        <v>1875</v>
+        <v>709</v>
       </c>
       <c r="N6" s="352" t="n">
-        <v>75</v>
+        <v>28.36</v>
       </c>
       <c r="O6" s="352" t="n">
-        <v>1950</v>
+        <v>737.36</v>
       </c>
       <c r="P6" s="352" t="n">
-        <v>599.1</v>
+        <v>184.34</v>
       </c>
       <c r="Q6" s="352" t="n">
-        <v>2549.1</v>
+        <v>921.7</v>
       </c>
       <c r="R6" s="352" t="n">
-        <v>17204.74</v>
+        <v>5657.82</v>
       </c>
     </row>
     <row r="7" ht="18.75" customHeight="1" s="334">
@@ -3769,48 +3763,48 @@
         </is>
       </c>
       <c r="C7" s="354" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D7" s="354" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="354" t="inlineStr"/>
       <c r="F7" s="354" t="n">
-        <v>18434</v>
+        <v>5672</v>
       </c>
       <c r="G7" s="354" t="inlineStr"/>
       <c r="H7" s="354" t="n">
-        <v>15000</v>
+        <v>5672</v>
       </c>
       <c r="I7" s="354" t="n">
-        <v>1800</v>
+        <v>680.64</v>
       </c>
       <c r="J7" s="354" t="n">
-        <v>138.26</v>
+        <v>42.54</v>
       </c>
       <c r="K7" s="354" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="354" t="n">
-        <v>1938.26</v>
+        <v>723.1799999999999</v>
       </c>
       <c r="M7" s="354" t="n">
-        <v>1875</v>
+        <v>709</v>
       </c>
       <c r="N7" s="354" t="n">
-        <v>75</v>
+        <v>28.36</v>
       </c>
       <c r="O7" s="354" t="n">
-        <v>1950</v>
+        <v>737.36</v>
       </c>
       <c r="P7" s="354" t="n">
-        <v>599.1</v>
+        <v>184.34</v>
       </c>
       <c r="Q7" s="354" t="n">
-        <v>2549.1</v>
+        <v>921.7</v>
       </c>
       <c r="R7" s="354" t="n">
-        <v>17204.74</v>
+        <v>5657.82</v>
       </c>
     </row>
     <row r="8" ht="18.75" customHeight="1" s="334">
@@ -3823,7 +3817,7 @@
         </is>
       </c>
       <c r="C8" s="352" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D8" s="352" t="n">
         <v>1</v>
@@ -3832,43 +3826,43 @@
         <v>589</v>
       </c>
       <c r="F8" s="352" t="n">
-        <v>15314</v>
+        <v>6479</v>
       </c>
       <c r="G8" s="352" t="n">
         <v>589</v>
       </c>
       <c r="H8" s="352" t="n">
-        <v>15000</v>
+        <v>6479</v>
       </c>
       <c r="I8" s="352" t="n">
-        <v>1800</v>
+        <v>777.48</v>
       </c>
       <c r="J8" s="352" t="n">
-        <v>114.85</v>
+        <v>48.59</v>
       </c>
       <c r="K8" s="352" t="n">
         <v>0</v>
       </c>
       <c r="L8" s="352" t="n">
-        <v>1914.85</v>
+        <v>826.0700000000001</v>
       </c>
       <c r="M8" s="352" t="n">
-        <v>1875</v>
+        <v>809.88</v>
       </c>
       <c r="N8" s="352" t="n">
-        <v>75</v>
+        <v>32.4</v>
       </c>
       <c r="O8" s="352" t="n">
-        <v>1950</v>
+        <v>842.28</v>
       </c>
       <c r="P8" s="352" t="n">
-        <v>497.71</v>
+        <v>210.57</v>
       </c>
       <c r="Q8" s="352" t="n">
-        <v>2447.71</v>
+        <v>1052.85</v>
       </c>
       <c r="R8" s="352" t="n">
-        <v>13988.15</v>
+        <v>6241.93</v>
       </c>
     </row>
     <row r="9" ht="18.75" customHeight="1" s="334">
@@ -3879,48 +3873,48 @@
         </is>
       </c>
       <c r="C9" s="354" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D9" s="354" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="354" t="inlineStr"/>
       <c r="F9" s="354" t="n">
-        <v>15314</v>
+        <v>6479</v>
       </c>
       <c r="G9" s="354" t="inlineStr"/>
       <c r="H9" s="354" t="n">
-        <v>15000</v>
+        <v>6479</v>
       </c>
       <c r="I9" s="354" t="n">
-        <v>1800</v>
+        <v>777.48</v>
       </c>
       <c r="J9" s="354" t="n">
-        <v>114.85</v>
+        <v>48.59</v>
       </c>
       <c r="K9" s="354" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="354" t="n">
-        <v>1914.85</v>
+        <v>826.0700000000001</v>
       </c>
       <c r="M9" s="354" t="n">
-        <v>1875</v>
+        <v>809.88</v>
       </c>
       <c r="N9" s="354" t="n">
-        <v>75</v>
+        <v>32.4</v>
       </c>
       <c r="O9" s="354" t="n">
-        <v>1950</v>
+        <v>842.28</v>
       </c>
       <c r="P9" s="354" t="n">
-        <v>497.71</v>
+        <v>210.57</v>
       </c>
       <c r="Q9" s="354" t="n">
-        <v>2447.71</v>
+        <v>1052.85</v>
       </c>
       <c r="R9" s="354" t="n">
-        <v>13988.15</v>
+        <v>6241.93</v>
       </c>
     </row>
     <row r="10" ht="18.75" customHeight="1" s="334">
@@ -3933,7 +3927,7 @@
         </is>
       </c>
       <c r="C10" s="352" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D10" s="352" t="n">
         <v>1</v>
@@ -3942,43 +3936,43 @@
         <v>504</v>
       </c>
       <c r="F10" s="352" t="n">
-        <v>13104</v>
+        <v>10584</v>
       </c>
       <c r="G10" s="352" t="n">
         <v>504</v>
       </c>
       <c r="H10" s="352" t="n">
-        <v>13104</v>
+        <v>10584</v>
       </c>
       <c r="I10" s="352" t="n">
-        <v>1572.48</v>
+        <v>1270.08</v>
       </c>
       <c r="J10" s="352" t="n">
-        <v>98.28</v>
+        <v>79.38</v>
       </c>
       <c r="K10" s="352" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="352" t="n">
-        <v>1670.76</v>
+        <v>1349.46</v>
       </c>
       <c r="M10" s="352" t="n">
-        <v>1638</v>
+        <v>1323</v>
       </c>
       <c r="N10" s="352" t="n">
-        <v>65.52</v>
+        <v>52.92</v>
       </c>
       <c r="O10" s="352" t="n">
-        <v>1703.52</v>
+        <v>1375.92</v>
       </c>
       <c r="P10" s="352" t="n">
-        <v>425.88</v>
+        <v>343.98</v>
       </c>
       <c r="Q10" s="352" t="n">
-        <v>2129.4</v>
+        <v>1719.9</v>
       </c>
       <c r="R10" s="352" t="n">
-        <v>11937.24</v>
+        <v>9738.540000000001</v>
       </c>
     </row>
     <row r="11" ht="18.75" customHeight="1" s="334">
@@ -3989,48 +3983,48 @@
         </is>
       </c>
       <c r="C11" s="354" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D11" s="354" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="354" t="inlineStr"/>
       <c r="F11" s="354" t="n">
-        <v>13104</v>
+        <v>10584</v>
       </c>
       <c r="G11" s="354" t="inlineStr"/>
       <c r="H11" s="354" t="n">
-        <v>13104</v>
+        <v>10584</v>
       </c>
       <c r="I11" s="354" t="n">
-        <v>1572.48</v>
+        <v>1270.08</v>
       </c>
       <c r="J11" s="354" t="n">
-        <v>98.28</v>
+        <v>79.38</v>
       </c>
       <c r="K11" s="354" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="354" t="n">
-        <v>1670.76</v>
+        <v>1349.46</v>
       </c>
       <c r="M11" s="354" t="n">
-        <v>1638</v>
+        <v>1323</v>
       </c>
       <c r="N11" s="354" t="n">
-        <v>65.52</v>
+        <v>52.92</v>
       </c>
       <c r="O11" s="354" t="n">
-        <v>1703.52</v>
+        <v>1375.92</v>
       </c>
       <c r="P11" s="354" t="n">
-        <v>425.88</v>
+        <v>343.98</v>
       </c>
       <c r="Q11" s="354" t="n">
-        <v>2129.4</v>
+        <v>1719.9</v>
       </c>
       <c r="R11" s="354" t="n">
-        <v>11937.24</v>
+        <v>9738.540000000001</v>
       </c>
     </row>
     <row r="12" ht="18.75" customHeight="1" s="334">
@@ -4041,48 +4035,48 @@
         </is>
       </c>
       <c r="C12" s="357" t="n">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D12" s="357" t="n">
         <v>3</v>
       </c>
       <c r="E12" s="357" t="inlineStr"/>
       <c r="F12" s="357" t="n">
-        <v>46852</v>
+        <v>22735</v>
       </c>
       <c r="G12" s="357" t="inlineStr"/>
       <c r="H12" s="357" t="n">
-        <v>43104</v>
+        <v>22735</v>
       </c>
       <c r="I12" s="357" t="n">
-        <v>5172.48</v>
+        <v>2728.2</v>
       </c>
       <c r="J12" s="357" t="n">
-        <v>351.39</v>
+        <v>170.51</v>
       </c>
       <c r="K12" s="357" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="357" t="n">
-        <v>5523.87</v>
+        <v>2898.71</v>
       </c>
       <c r="M12" s="357" t="n">
-        <v>5388</v>
+        <v>2841.88</v>
       </c>
       <c r="N12" s="357" t="n">
-        <v>215.52</v>
+        <v>113.68</v>
       </c>
       <c r="O12" s="357" t="n">
-        <v>5603.52</v>
+        <v>2955.56</v>
       </c>
       <c r="P12" s="357" t="n">
-        <v>1522.69</v>
+        <v>738.89</v>
       </c>
       <c r="Q12" s="357" t="n">
-        <v>7126.209999999999</v>
+        <v>3694.45</v>
       </c>
       <c r="R12" s="357" t="n">
-        <v>43130.13</v>
+        <v>21638.29</v>
       </c>
     </row>
     <row r="16">
@@ -4250,13 +4244,13 @@
         <v>504</v>
       </c>
       <c r="D8" s="290" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E8" s="290" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F8" s="291" t="n">
-        <v>13104</v>
+        <v>10584</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="334">
@@ -4272,13 +4266,13 @@
         <v>589</v>
       </c>
       <c r="D9" s="290" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E9" s="290" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F9" s="291" t="n">
-        <v>15314</v>
+        <v>6479</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="334">
@@ -4294,13 +4288,13 @@
         <v>709</v>
       </c>
       <c r="D10" s="290" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E10" s="290" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F10" s="291" t="n">
-        <v>18434</v>
+        <v>5672</v>
       </c>
     </row>
     <row r="11" ht="26.25" customHeight="1" s="334">
@@ -4430,7 +4424,7 @@
       <c r="D16" s="290" t="n"/>
       <c r="E16" s="290" t="n"/>
       <c r="F16" s="291" t="n">
-        <v>5388</v>
+        <v>2841.88</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="334">
@@ -4448,7 +4442,7 @@
       <c r="D17" s="290" t="n"/>
       <c r="E17" s="290" t="n"/>
       <c r="F17" s="291" t="n">
-        <v>1522.69</v>
+        <v>738.89</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="334">
@@ -4466,7 +4460,7 @@
       <c r="D18" s="290" t="n"/>
       <c r="E18" s="290" t="n"/>
       <c r="F18" s="291" t="n">
-        <v>215.52</v>
+        <v>113.68</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="334">
@@ -4496,7 +4490,7 @@
       <c r="D20" s="290" t="n"/>
       <c r="E20" s="290" t="n"/>
       <c r="F20" s="291" t="n">
-        <v>1824.68</v>
+        <v>886.41</v>
       </c>
       <c r="G20" s="295" t="n"/>
     </row>
@@ -4515,7 +4509,7 @@
       <c r="D21" s="290" t="n"/>
       <c r="E21" s="290" t="n"/>
       <c r="F21" s="291" t="n">
-        <v>10368.8802</v>
+        <v>5241.2148</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="334">
@@ -4533,7 +4527,7 @@
       <c r="D22" s="290" t="n"/>
       <c r="E22" s="290" t="n"/>
       <c r="F22" s="291" t="n">
-        <v>67973.7702</v>
+        <v>34359.0748</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="334">
@@ -4649,7 +4643,7 @@
       <c r="D28" s="289" t="n"/>
       <c r="E28" s="289" t="n"/>
       <c r="F28" s="298" t="n">
-        <v>67973.7702</v>
+        <v>34359.0748</v>
       </c>
     </row>
     <row r="29" ht="39" customHeight="1" s="334">

</xml_diff>